<commit_message>
new excel template (Input Template-Exec.xls) added
</commit_message>
<xml_diff>
--- a/test/input/Empty.xlsx
+++ b/test/input/Empty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="208" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="141" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,15 +17,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Peer Group</t>
-  </si>
-  <si>
-    <t>Founding Year</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -119,28 +155,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="A2:C6"/>
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -162,11 +240,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A2:C6 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -187,11 +265,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A2:C6 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>